<commit_message>
Added message when submitting (new) student
</commit_message>
<xml_diff>
--- a/Planning en Documentatie/SprintBacklog.xlsx
+++ b/Planning en Documentatie/SprintBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JustFalco\Documents\Development\Github desktop\Eindcase traineeship\TraineeshipEindcase\Planning en Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2FC0BE1-4CB7-40C1-8A40-D5A36871E66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC2CBB5-D3E0-4912-B19F-E1FBDA9578C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1440" windowWidth="29040" windowHeight="18240" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,15 +604,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,11 +663,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -782,15 +770,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -855,8 +842,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,12 +903,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
     <cellStyle name="Goed" xfId="4" builtinId="26"/>
-    <cellStyle name="Neutraal" xfId="5" builtinId="28"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1289,11 +1273,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1337,14 +1321,14 @@
       <c r="AH2"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1437,11 +1421,11 @@
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
@@ -1465,9 +1449,9 @@
       <c r="AJ8" s="4"/>
     </row>
     <row r="9" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
       <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
@@ -1493,11 +1477,11 @@
       <c r="AJ10" s="20"/>
     </row>
     <row r="11" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="I11" s="17" t="s">
         <v>38</v>
       </c>
@@ -1515,9 +1499,9 @@
       <c r="AJ11" s="4"/>
     </row>
     <row r="12" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="I12" s="7" t="s">
         <v>39</v>
       </c>
@@ -1535,9 +1519,9 @@
       <c r="AJ12" s="4"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
       <c r="J13" s="4"/>
       <c r="W13"/>
       <c r="X13"/>
@@ -1546,9 +1530,9 @@
       <c r="AJ13" s="4"/>
     </row>
     <row r="14" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
       <c r="J14" s="4"/>
       <c r="S14" s="17" t="s">
         <v>27</v>
@@ -1563,11 +1547,11 @@
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
       <c r="J15" s="4"/>
-      <c r="S15" s="44" t="s">
+      <c r="S15" s="42" t="s">
         <v>83</v>
       </c>
       <c r="U15" s="8" t="s">
@@ -1582,16 +1566,16 @@
     <row r="16" spans="1:36" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="S16" s="45"/>
+      <c r="S16" s="43"/>
       <c r="AI16" s="20"/>
       <c r="AJ16" s="20"/>
     </row>
     <row r="17" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="I17" s="17" t="s">
         <v>48</v>
       </c>
@@ -1603,9 +1587,9 @@
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
       <c r="I18" s="8" t="s">
         <v>49</v>
       </c>
@@ -1617,9 +1601,9 @@
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="W19"/>
@@ -1629,9 +1613,9 @@
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
       <c r="G20" s="17" t="s">
         <v>56</v>
       </c>
@@ -1646,9 +1630,9 @@
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
       <c r="G21" s="7"/>
       <c r="I21" s="8" t="s">
         <v>58</v>
@@ -1661,9 +1645,9 @@
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="W22"/>
@@ -1673,9 +1657,9 @@
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
       <c r="G23" s="17" t="s">
         <v>80</v>
       </c>
@@ -1688,9 +1672,9 @@
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
       <c r="G24" s="8" t="s">
         <v>81</v>
       </c>
@@ -1728,11 +1712,11 @@
       <c r="AJ25" s="20"/>
     </row>
     <row r="26" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
       <c r="G26" s="17" t="s">
         <v>64</v>
       </c>
@@ -1751,9 +1735,9 @@
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
       <c r="G27" s="7"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1776,11 +1760,11 @@
       <c r="AJ28" s="20"/>
     </row>
     <row r="29" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="J29" s="4"/>
       <c r="W29" s="17" t="s">
         <v>8</v>
@@ -1797,9 +1781,9 @@
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
       <c r="J30" s="4"/>
       <c r="W30" s="8" t="s">
         <v>30</v>
@@ -1815,9 +1799,9 @@
       <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="I32" s="17" t="s">
         <v>70</v>
       </c>
@@ -1828,9 +1812,9 @@
       <c r="AH32" s="4"/>
     </row>
     <row r="33" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
       <c r="I33" s="8" t="s">
         <v>71</v>
       </c>
@@ -1841,9 +1825,9 @@
       <c r="AH33" s="4"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -1862,9 +1846,9 @@
       <c r="AH34" s="4"/>
     </row>
     <row r="35" spans="1:34" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
       <c r="K35" s="17" t="s">
         <v>8</v>
       </c>
@@ -1881,9 +1865,9 @@
       <c r="AH35" s="4"/>
     </row>
     <row r="36" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
       <c r="K36" s="8" t="s">
         <v>30</v>
       </c>
@@ -2186,7 +2170,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:G17"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,16 +2683,16 @@
       <c r="C20" s="21">
         <v>3</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="21" t="s">
         <v>23</v>
       </c>
@@ -2749,16 +2733,16 @@
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="22" t="s">
         <v>42</v>
       </c>
       <c r="H22" t="s">

</xml_diff>